<commit_message>
xlsx or xls read, translate, write success with Google/SYSTRAN  Translator: row and column numbers are taken from the file automatically and phone numbers, dates and email are translated properly.
</commit_message>
<xml_diff>
--- a/SourceSampleForTesting.xlsx
+++ b/SourceSampleForTesting.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZipZap\Desktop\intelliJ Projects\ExcelTranslationProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D53725E-3E6B-4948-928F-083C54E6AC1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF7D399-8B0B-4049-96A8-03C9DAFAD30E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="1890" windowWidth="25725" windowHeight="14310" xr2:uid="{4C0F71E9-9613-47D0-A3E4-E2778290887D}"/>
+    <workbookView xWindow="2175" yWindow="345" windowWidth="25350" windowHeight="14310" xr2:uid="{4C0F71E9-9613-47D0-A3E4-E2778290887D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="97">
   <si>
     <t>序号</t>
   </si>
@@ -195,9 +195,6 @@
     <t>2020-06-04</t>
   </si>
   <si>
-    <t>0998-2597999</t>
-  </si>
-  <si>
     <t>1601757779@qq.com</t>
   </si>
   <si>
@@ -271,13 +268,70 @@
   </si>
   <si>
     <t>lannyzg16019@qq.com</t>
+  </si>
+  <si>
+    <t>日用百货销售；厨具卫具及日用杂品批发；家用电器销售；机械设备销售；塑料制品销售；农、林、牧、副、渔业专业机械的销售；农业机械销售；农产品的生产、销售、加工、运输、贮藏及其他相关服务；牲畜销售；林木种子生产经营；树木种植经营；食用农产品批发；文具用品批发；体育用品及器材批发；乐器批发；游艺及娱乐用品销售；煤炭及制品销售；第一类医疗器械销售；食品经营（销售预包装食品）；第二类医疗器械销售；建筑材料销售；汽车零配件批发；新能源汽车整车销售；新能源汽车电附件销售；摩托车及零配件批发；五金产品批发；计算机软硬件及辅助设备批发；电气设备销售；通讯设备销售；广播影视设备销售；金属制品销售；办公设备销售；仪器仪表销售；消防器材销售；智能农机装备销售；生态环境监测及检测仪器仪表销售；医用口罩批发；日用口罩（非医用）销售；消毒剂销售（不含危险化学品）；卫生用品和一次性使用医疗用品销售；特种劳动防护用品销售；劳动保护用品销售；新鲜水果批发；电线、电缆经营；家具零配件销售；技术服务、技术开发、技术咨询、技术交流、技术转让、技术推广；家居用品销售；家用电器零配件销售；汽车新车销售；建筑装饰材料销售；机械零件、零部件销售；农作物种子经营（仅限不再分装的包装种子）；环境保护专用设备销售；汽车装饰用品销售；农林牧渔机械配件销售；建筑工程用机械销售；教学专用仪器销售；畜牧机械销售；草及相关制品销售；建筑用钢筋产品销售；电子产品销售；办公设备耗材销售；软件销售；水泥制品销售；饲料生产专用设备销售；办公用品销售；安防设备销售；牲畜销售（不含犬类）；汽车零配件零售；通信设备销售；五金产品零售；家具销售；酒类经营；玩具销售；警用装备销售（须公安机关认定资格）；安防设备制造；特种设备销售；广告制作；广告设计、代理；消防技术服务；建筑工程机械与设备租赁；建筑劳务分包；土石方工程施工；对外承包工程；园林绿化工程施工；各类工程建设活动；消防设施工程施工；房屋建筑和市政基础设施项目工程总承包</t>
+  </si>
+  <si>
+    <t>和田德军商贸有限公司</t>
+  </si>
+  <si>
+    <t>姚可利</t>
+  </si>
+  <si>
+    <t>100万(元)</t>
+  </si>
+  <si>
+    <t>2021-05-08</t>
+  </si>
+  <si>
+    <t>和田地区</t>
+  </si>
+  <si>
+    <t>策勒县</t>
+  </si>
+  <si>
+    <t>新疆和田地区策勒县固拉合玛镇创业市场1号楼5-6号</t>
+  </si>
+  <si>
+    <t>和田亿丰实业有限公司</t>
+  </si>
+  <si>
+    <t>解焕忠</t>
+  </si>
+  <si>
+    <t>380万(元)</t>
+  </si>
+  <si>
+    <t>2020-05-08</t>
+  </si>
+  <si>
+    <t>15199242666</t>
+  </si>
+  <si>
+    <t>78124667@qq.com</t>
+  </si>
+  <si>
+    <t>墨玉县</t>
+  </si>
+  <si>
+    <t>新疆和田地区墨玉县博斯坦管委会博斯坦库勒工业园区香山路20号</t>
+  </si>
+  <si>
+    <t>牲畜屠宰；家禽屠宰；畜牧业经营；农业经营；畜牧业专业及辅助性服务；农业专业及辅助性服务；食用农产品购销；农产品初加工；五金产品批发；办公设备销售；日用百货销售；集贸市场管理服务；金属材料销售；化妆品批发；气体、液体分离及纯净设备销售；食品用塑料包装容器工具制品销售；包装专用设备销售；建筑材料销售；电子产品销售；机械设备销售；日用木制品销售；塑料制品销售；玻璃纤维增强塑料制品销售；建筑装饰材料销售；劳动保护用品销售；制冷、空调设备销售；通用设备修理；电子专用设备销售；家用电器零配件销售；环境保护专用设备销售；发电机及发电机组销售；建筑工程用机械销售；农业机械销售；特种设备销售；计算器设备销售；电力设施器材销售；农副食品加工专用设备销售；机械零件、零部件销售；会议及展览服务；风机、风扇销售；光通信设备销售；通信设备销售；金属工具销售；专用化学产品销售（不含危险化学品）；医疗设备租赁；实验分析仪器制造；办公设备租赁服务；计算机及办公设备维修；办公服务；办公设备耗材销售；文具用品零售；图文设计制作；家具制造；文具用品批发；体育用品及器材零售；家具销售；涂料销售（不含危险化学品）；计算机系统服务；机械设备租赁；广告设计、代理；广告制作；平面设计；广告发布（非广播电台、电视台、报刊出版单位）；品牌管理；建筑用石加工；门窗制造加工；建筑防水卷材产品制造；建筑防水卷材产品销售；建筑工程机械与设备租赁；建筑装饰、水暖管道零件及其他建筑用金属制品制造；建筑物清洁服务；园林绿化工程施工；体育场地设施工程施工；土石方工程施工；金属门窗工程施工；卫生洁具销售；食用农产品初加工；初级农产品收购；通讯设备销售；固体废物治理；土地整治服务；房屋拆迁服务；金属结构销售；建筑用钢筋产品销售；普通机械设备安装服务；矿物洗选加工；铸造用造型材料销售；互联网销售（除销售需要许可的商品）；实验分析仪器销售；服装服饰零售；汽车零配件批发；软件开发；茶具销售；农副产品销售；消毒剂销售（不含危险化学品）；食用农产品零售；针纺织品及原料销售；第一类医疗器械销售；新鲜蔬菜批发；水产品批发；针纺织品销售；家居用品销售；新鲜水果零售；谷物销售；第二类医疗器械销售；国内贸易代理；食品经营（仅销售预包装食品）；未经加工的坚果、干果销售（依法须经批准的项目，经相关部门批准后方可开展经营活动）</t>
+  </si>
+  <si>
+    <t>日用百货销售；厨具卫具及日用杂品批发；家用电器销售；机械设备销售；塑料制品销售；农、林、牧、副、渔业专业机械的销售；农业机械销售；农产品的生产、销售、加工、运输、贮藏及其他相关服务；牲畜销售；林木种子生产经营；树木种植经营；食用农产品批发；文具用品批发；体育用品及器材批发；乐器批发；游艺及娱乐用品销售；煤炭及制品销售；第一类医疗器械销售；食品经营（销售预包装食品）；第二类医疗器械销售；建筑材料销售；汽车零配件批发；新能源汽车整车销售；新能源汽车电附件销售；摩托车及零配件批发；五金产品批发；计算机软硬件及辅助设备批发；电气设备销售；通讯设备销售；广播影视设备销售；金属制品销售；办公设备销售；仪器仪表销售；消防器材销售；智能农机装备销售；生态环境监测及检测仪器仪表销售；医用口罩批发；日用口罩（非医用）销售；消毒剂销售（不含危险化学品）；卫生用品和一次性使用医疗用品销售；特种劳动防护用品销售；劳动保护用品销售；新鲜水果批发；电线、电缆经营；家具零配件销售；技术服务、技术开发、技术咨询、技术交流、技术转让、技术推广；家居用品销售；家用电器零配件销售；汽车新车销售；建筑装饰材料销售；机械零件、零部件销售；农作物种子经营（仅限不再分装的包装种子）；环境保护专用设备销售；汽车装饰用品销售；农林牧渔机械配件销售；建筑工程用机械销售；教学专用仪器销售；畜牧机械销售；草及相关制品销售；建筑用钢筋产品销售；电子产品销售；办公设备耗材销售；软件销售；水泥制品销售；饲料生产专用设备销售；办公用品销售；安防设备销售；牲畜销售（不含犬类）；汽车零配件零售；通信设备销售；五金产品零售；家具销售；酒类经营；玩具销售；警用装备销售（须公安机关认定资格）；安防设备制造；特种设备销售；广告制作；广告设计、代理；消防技术服务；建筑工程机械与设备租赁；建筑劳务分包；土石方工程施工；对外承包工程；园林绿化工程施工；各类工程建设活动；消防设施工程施工；房屋建筑和市政基础设施项目工程总承包 牲畜屠宰；家禽屠宰；畜牧业经营；农业经营；畜牧业专业及辅助性服务；农业专业及辅助性服务；食用农产品购销；农产品初加工；五金产品批发；办公设备销售；日用百货销售；集贸市场管理服务；金属材料销售；化妆品批发；气体、液体分离及纯净设备销售；食品用塑料包装容器工具制品销售；包装专用设备销售；建筑材料销售；电子产品销售；机械设备销售；日用木制品销售；塑料制品销售；玻璃纤维增强塑料制品销售；建筑装饰材料销售；劳动保护用品销售；制冷、空调设备销售；通用设备修理；电子专用设备销售；家用电器零配件销售；环境保护专用设备销售；发电机及发电机组销售；建筑工程用机械销售；农业机械销售；特种设备销售；计算器设备销售；电力设施器材销售；农副食品加工专用设备销售；机械零件、零部件销售；会议及展览服务；风机、风扇销售；光通信设备销售；通信设备销售；金属工具销售；专用化学产品销售（不含危险化学品）；医疗设备租赁；实验分析仪器制造；办公设备租赁服务；计算机及办公设备维修；办公服务；办公设备耗材销售；文具用品零售；图文设计制作；家具制造；文具用品批发；体育用品及器材零售；家具销售；涂料销售（不含危险化学品）；计算机系统服务；机械设备租赁；广告设计、代理；广告制作；平面设计；广告发布（非广播电台、电视台、报刊出版单位）；品牌管理；建筑用石加工；门窗制造加工；建筑防水卷材产品制造；建筑防水卷材产品销售；建筑工程机械与设备租赁；建筑装饰、水暖管道零件及其他建筑用金属制品制造；建筑物清洁服务；园林绿化工程施工；体育场地设施工程施工；土石方工程施工；金属门窗工程施工；卫生洁具销售；食用农产品初加工；初级农产品收购；通讯设备销售；固体废物治理；土地整治服务；房屋拆迁服务；金属结构销售；建筑用钢筋产品销售；普通机械设备安装服务；矿物洗选加工；铸造用造型材料销售；互联网销售（除销售需要许可的商品）；实验分析仪器销售；服装服饰零售；汽车零配件批发；软件开发；茶具销售；农副产品销售；消毒剂销售（不含危险化学品）；食用农产品零售；针纺织品及原料销售；第一类医疗器械销售；新鲜蔬菜批发；水产品批发；针纺织品销售；家居用品销售；新鲜水果零售；谷物销售；第二类医疗器械销售；国内贸易代理；食品经营（仅销售预包装食品）；未经加工的坚果、干果销售（依法须经批准的项目，经相关部门批准后方可开展经营活动）                                            一般项目：钢压延加工；有色金属压延加工；金属切削加工服务；建筑工程用机械制造；金属加工机械制造；建筑工程用机械销售；农业机械制造；农业机械租赁；农业机械服务；专用设备制造（不含许可类专业设备制造）；金属结构制造；金属结构销售；建筑工程机械与设备租赁；机械设备租赁；机械设备销售；烘炉、熔炉及电炉制造；烘炉、熔炉及电炉销售；电力设施器材制造；机械电气设备制造；机械电气设备销售；环境保护专用设备制造；环境保护专用设备销售；物料搬运装备制造；物料搬运装备销售；电容器及其配套设备制造；电容器及其配套设备销售；木制容器销售；木制容器制造；金属包装容器及材料销售；金属包装容器及材料制造；建筑材料生产专用机械制造；建筑用钢筋产品销售；建筑用金属配件销售；建筑用金属配件制造；承接总公司工程建设业务；砼结构构件销售；建筑装饰、水暖管道零件及其他建筑用金属制品制造；建筑装饰材料销售；门窗销售；工程管理服务；安全咨询服务；管道运输设备销售；普通机械设备安装服务；电子、机械设备维护（不含特种设备）；运输设备租赁服务；计算机及通讯设备租赁；特种设备出租；通用设备修理；专用设备修理；电气设备修理；通讯设备修理；金属材料销售；金属材料制造；电气设备销售；电器辅件销售；有色金属合金销售；电子专用材料销售；电子专用设备销售；电子专用设备制造；五金产品批发；五金产品制造；五金产品零售；泵及真空设备销售；建筑材料销售；轻质建筑材料销售；建筑防水卷材产品销售；阀门和旋塞销售；劳动保护用品销售；普通货物仓储服务（不含危险化学品等需许可审批的项目）；特种设备销售；通用设备制造（不含特种设备制造）；金属成形机床销售；金属成形机床制造。（除依法须经批准的项目外，凭营业执照依法自主开展经营活动）</t>
+  </si>
+  <si>
+    <t>和田亿丰公司 (组合示例)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -311,8 +365,16 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -334,6 +396,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -390,11 +458,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyFill="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -421,9 +490,28 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{DF62752C-7E0C-4D5A-933F-4B7BA9A0A655}"/>
   </cellStyles>
@@ -737,10 +825,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F03795-681A-499A-9381-8EB2667CF0C0}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E7" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -796,7 +884,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="3" customFormat="1" ht="120.75">
+    <row r="2" spans="1:12" s="3" customFormat="1" ht="60" customHeight="1">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -816,7 +904,7 @@
         <v>15999018373</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>17</v>
@@ -834,7 +922,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="3" customFormat="1" ht="86.25">
+    <row r="3" spans="1:12" s="3" customFormat="1" ht="61.5" customHeight="1">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -877,16 +965,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>73</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>30</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>16</v>
@@ -895,7 +983,7 @@
         <v>16</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I4" s="8" t="s">
         <v>16</v>
@@ -904,10 +992,10 @@
         <v>33</v>
       </c>
       <c r="K4" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="L4" s="9" t="s">
         <v>76</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="3" customFormat="1" ht="51.75">
@@ -1040,11 +1128,11 @@
       <c r="E8" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="4">
+        <v>9982597999</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>17</v>
@@ -1056,10 +1144,10 @@
         <v>33</v>
       </c>
       <c r="K8" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="L8" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="3" customFormat="1" ht="276">
@@ -1067,37 +1155,37 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>58</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>38</v>
       </c>
       <c r="E9" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>17</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>33</v>
       </c>
       <c r="K9" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="L9" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="3" customFormat="1" ht="34.5">
@@ -1105,42 +1193,157 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>66</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>38</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F10" s="4">
         <v>15999018373</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>17</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>33</v>
       </c>
       <c r="K10" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="L10" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="L10" s="5" t="s">
-        <v>71</v>
+    </row>
+    <row r="11" spans="1:12" ht="362.25">
+      <c r="A11" s="11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="409.5">
+      <c r="A12" s="12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="J12" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="L12" s="16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="409.5">
+      <c r="A13" s="12">
+        <v>12</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="J13" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="K13" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="L13" s="16" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G10" r:id="rId1" xr:uid="{781BC18A-2A01-4FE3-A253-D86DB8D0458C}"/>
+    <hyperlink ref="G2" r:id="rId2" xr:uid="{F9B09D86-B6C5-4A1F-BC5B-C6DEBDE45038}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>